<commit_message>
Update Exec13 upr 1, 2, 4
</commit_message>
<xml_diff>
--- a/БюджетДекабрь.xlsx
+++ b/БюджетДекабрь.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Поступления</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Васе подарок др</t>
+  </si>
+  <si>
+    <t>ЗП</t>
+  </si>
+  <si>
+    <t>Ипотека</t>
+  </si>
+  <si>
+    <t>Доскрочка</t>
   </si>
 </sst>
 </file>
@@ -482,14 +491,14 @@
   <dimension ref="A2:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="3.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" customWidth="1"/>
@@ -511,7 +520,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="3">
         <f>G4+K4+O4+S4</f>
-        <v>17238.48</v>
+        <v>48799.48</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>20</v>
@@ -519,7 +528,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="3">
         <f>C3-G2</f>
-        <v>21671.52</v>
+        <v>31482.379999999997</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -529,7 +538,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="1">
         <f>SUM(C4:C18)</f>
-        <v>38910</v>
+        <v>80281.86</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -556,12 +565,12 @@
       <c r="J4" s="6"/>
       <c r="K4" s="3">
         <f>SUM(K5:K18)</f>
-        <v>9000</v>
-      </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3" t="s">
+        <v>40561</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="N4" s="6"/>
       <c r="O4" s="3">
         <f>SUM(O5:O18)</f>
         <v>6156.5</v>
@@ -623,9 +632,15 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="2">
+        <v>44924</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3">
+        <v>41371.86</v>
+      </c>
       <c r="E6" s="2">
         <v>44920</v>
       </c>
@@ -670,9 +685,15 @@
       <c r="G7" s="3">
         <v>64</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="I7" s="2">
+        <v>44924</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="3">
+        <v>16561</v>
+      </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
         <v>8</v>
@@ -704,8 +725,12 @@
         <v>64</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="3">
+        <v>15000</v>
+      </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3" t="s">
         <v>9</v>
@@ -993,13 +1018,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>